<commit_message>
first batch of participants
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Desktop/wtp_rej_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melanieruiz/Documents/GitHub/WTP_Rejection_Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC34F93C-A07F-BA4A-909F-21EA4A69A1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5EE4A3-7899-1540-8FC8-81C11D1EF6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="500" windowWidth="36380" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3720" yWindow="1080" windowWidth="17280" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>pavlovia_task</t>
   </si>
@@ -55,15 +55,9 @@
     <t>Initials</t>
   </si>
   <si>
-    <t>JSD</t>
-  </si>
-  <si>
     <t>pretasksub_id</t>
   </si>
   <si>
-    <t>R_2wieTt2vepP7fRw</t>
-  </si>
-  <si>
     <t>R_10VrT1bZzlTkiIS</t>
   </si>
   <si>
@@ -124,7 +118,52 @@
     <t>Other</t>
   </si>
   <si>
-    <t>test_0410</t>
+    <t>n</t>
+  </si>
+  <si>
+    <t>60fc66800ccfce9c74ed4f3d</t>
+  </si>
+  <si>
+    <t>5e6027f12036113753519c82</t>
+  </si>
+  <si>
+    <t>65779c4bde34621ce896b77d</t>
+  </si>
+  <si>
+    <t>5fab3afc780978629141d35f</t>
+  </si>
+  <si>
+    <t>60fe49ad235696796d15f22f</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>R_71QRzOCf6SCyykG</t>
+  </si>
+  <si>
+    <t>R_3OW5qJ9BiLi9fLx</t>
+  </si>
+  <si>
+    <t>R_3IaEV0ozOrhbwm7</t>
+  </si>
+  <si>
+    <t>R_5PdmG0TTITkHEy1</t>
+  </si>
+  <si>
+    <t>R_6n8bZLFNhTTYY2S</t>
+  </si>
+  <si>
+    <t>R_6qTjvQH3gV5cOTn</t>
+  </si>
+  <si>
+    <t>R_5plGE6TsnsUQcrv</t>
+  </si>
+  <si>
+    <t>R_7ZQZ79T1AysxFwx</t>
+  </si>
+  <si>
+    <t>R_1YahCCp8wSq4NYv</t>
   </si>
 </sst>
 </file>
@@ -203,9 +242,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -217,6 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,13 +477,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="180" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -455,19 +492,19 @@
     <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="4" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="11" customWidth="1"/>
+    <col min="6" max="6" width="19" style="10" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" customWidth="1"/>
-    <col min="10" max="10" width="21.1640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" style="8" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" customWidth="1"/>
     <col min="12" max="12" width="26" customWidth="1"/>
     <col min="13" max="13" width="14.83203125" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="11" customWidth="1"/>
+    <col min="14" max="14" width="19.5" style="10" customWidth="1"/>
     <col min="15" max="15" width="19.5" customWidth="1"/>
     <col min="16" max="16" width="15.1640625" customWidth="1"/>
     <col min="17" max="17" width="16" customWidth="1"/>
-    <col min="18" max="18" width="103.33203125" style="13" customWidth="1"/>
+    <col min="18" max="18" width="103.33203125" style="12" customWidth="1"/>
     <col min="19" max="22" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -476,102 +513,102 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>13</v>
+      <c r="F1" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="5">
-        <v>44873</v>
+        <v>45393</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="11">
-        <v>44872</v>
+        <v>28</v>
+      </c>
+      <c r="F2" s="10">
+        <v>45393</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>3</v>
+      <c r="J2" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -579,12 +616,12 @@
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="10">
         <v>44875</v>
       </c>
       <c r="O2">
         <f>_xlfn.DAYS(N2,F2)</f>
-        <v>3</v>
+        <v>-518</v>
       </c>
       <c r="P2" s="6">
         <v>2</v>
@@ -592,8 +629,8 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2" s="13" t="s">
-        <v>12</v>
+      <c r="R2" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="S2" s="4">
         <v>0</v>
@@ -608,7 +645,111 @@
         <v>3</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45393</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="10">
+        <v>45393</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5">
+        <v>45393</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="10">
+        <v>45393</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="5">
+        <v>45393</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="10">
+        <v>45393</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5">
+        <v>45393</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="10">
+        <v>45393</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LL_data for 11 participants
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordansiegel/Documents/GitHub/WTP_Rejection_Choice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farerilab/Documents/GitHub/WTP_Rejection_Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF740A64-FA9E-AC4E-AB11-1B537F81200E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891EE0CE-8D0B-4D47-B5BE-07F882C075F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1600" windowWidth="21460" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="320" yWindow="1700" windowWidth="30380" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId1"/>
@@ -18,25 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pilottotalparticipant_list!$K$1:$K$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="148">
   <si>
     <t>pavlovia_task</t>
   </si>
@@ -384,6 +371,102 @@
   </si>
   <si>
     <t>6098a486fc0e4c5db3a08e71</t>
+  </si>
+  <si>
+    <t>R_7fB3VBsN8UQsGNE</t>
+  </si>
+  <si>
+    <t>R_5hX4VmeqRXfwzkV</t>
+  </si>
+  <si>
+    <t>R_5U3jZRCu0AIsEiy</t>
+  </si>
+  <si>
+    <t>R_6tMd3Bw60rm9r0E</t>
+  </si>
+  <si>
+    <t>R_396cwo3bleOFgSN</t>
+  </si>
+  <si>
+    <t>R_55kobmsELxhtuKJ</t>
+  </si>
+  <si>
+    <t>R_7NEbXIzaHEzcgMu</t>
+  </si>
+  <si>
+    <t>R_1d5ZuATUJ4llxM5</t>
+  </si>
+  <si>
+    <t>R_7H3EM6hSwhQvEjL</t>
+  </si>
+  <si>
+    <t>R_6YGhwa797CuGY6t</t>
+  </si>
+  <si>
+    <t>R_1CHsBKT2rwXGGeN</t>
+  </si>
+  <si>
+    <t>R_6rD8nXK1PCdCPD7</t>
+  </si>
+  <si>
+    <t>R_7U9JCwAm8tY0f60</t>
+  </si>
+  <si>
+    <t>duplicte response in pretask- using first response</t>
+  </si>
+  <si>
+    <t>R_5LCFdgd87jHPGMF</t>
+  </si>
+  <si>
+    <t>R_6Lm2ZE8S01m3Tvb</t>
+  </si>
+  <si>
+    <t>R_5aEvnWyJjopL3Ke</t>
+  </si>
+  <si>
+    <t>R_3YRfd2rUdNI8UkV</t>
+  </si>
+  <si>
+    <t>R_65itrw5jYKKAGL7</t>
+  </si>
+  <si>
+    <t>R_7lJHxa6bkFILe9K</t>
+  </si>
+  <si>
+    <t>R_57GVI7klsFed12V</t>
+  </si>
+  <si>
+    <t>R_7xAjKzLEuQvL48m</t>
+  </si>
+  <si>
+    <t>R_3y3Y7kqtnKXXjCO</t>
+  </si>
+  <si>
+    <t>R_7uwvd79qgXhAE6A</t>
+  </si>
+  <si>
+    <t>R_5ScGrwQmxloyS2J</t>
+  </si>
+  <si>
+    <t>R_6PCetY961P9o5Ld</t>
+  </si>
+  <si>
+    <t>R_5tVXV2vKfvzuFEt</t>
+  </si>
+  <si>
+    <t>photo 9 was alcohol- replaced with photo 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uploading picture from different accounts </t>
+  </si>
+  <si>
+    <t>uplaoded pictures from instagram app instead of browser, repaced photo 12 (alcohol) with photo 26, replaced photo 21 with photo 27</t>
+  </si>
+  <si>
+    <t>photo 5 was a gif, replaced with photo 26; uploaded pictures from instagram app instead of internet browser, neds two more social experiences</t>
+  </si>
+  <si>
+    <t>getting more experiences</t>
   </si>
 </sst>
 </file>
@@ -450,7 +533,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,6 +552,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -482,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -532,6 +621,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,10 +849,10 @@
   <dimension ref="A1:X37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="180" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1632,74 +1723,392 @@
       </c>
     </row>
     <row r="25" spans="1:19" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" t="s">
+        <v>142</v>
+      </c>
       <c r="C25" s="16"/>
+      <c r="D25" s="33" t="s">
+        <v>116</v>
+      </c>
       <c r="E25" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="K25" s="31"/>
+      <c r="F25" s="34">
+        <v>45475.893946759257</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="31" t="s">
+        <v>27</v>
+      </c>
       <c r="O25" s="17"/>
       <c r="S25" s="32"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C26" s="5"/>
+      <c r="A26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="5">
+        <v>45476</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>123</v>
+      </c>
       <c r="E26" s="29" t="s">
         <v>104</v>
       </c>
+      <c r="F26" s="34">
+        <v>45475.933194444442</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S26" s="12" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" s="5">
+        <v>45476</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>117</v>
+      </c>
       <c r="E27" s="28" t="s">
         <v>105</v>
       </c>
+      <c r="F27" s="34">
+        <v>45475.898773148147</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="5">
+        <v>45477</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>118</v>
+      </c>
       <c r="E28" s="28" t="s">
         <v>106</v>
       </c>
+      <c r="F28" s="34">
+        <v>45475.899189814816</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S28" s="12" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="5">
+        <v>45478</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>119</v>
+      </c>
       <c r="E29" s="28" t="s">
         <v>107</v>
       </c>
+      <c r="F29" s="34">
+        <v>45475.907094907408</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" s="5">
+        <v>45479</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>120</v>
+      </c>
       <c r="E30" s="28" t="s">
         <v>108</v>
       </c>
+      <c r="F30" s="34">
+        <v>45475.912314814814</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="S30" s="12" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="5">
+        <v>45480</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>121</v>
+      </c>
       <c r="E31" s="28" t="s">
         <v>109</v>
       </c>
+      <c r="F31" s="34">
+        <v>45475.918715277781</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S31" s="12" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="5">
+        <v>45481</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>128</v>
+      </c>
       <c r="E32" s="28" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="33" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F32" s="34">
+        <v>45475.990833333337</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="S32" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="5">
+        <v>45482</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>126</v>
+      </c>
       <c r="E33" s="28" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="34" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F33" s="34">
+        <v>45476.090590277781</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="5">
+        <v>45483</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>127</v>
+      </c>
       <c r="E34" s="28" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="35" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F34" s="34">
+        <v>45476.23265046296</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" s="5">
+        <v>45484</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>124</v>
+      </c>
       <c r="E35" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="36" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F35" s="34">
+        <v>45475.935532407406</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="5">
+        <v>45485</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>122</v>
+      </c>
       <c r="E36" s="28" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="37" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F36" s="34">
+        <v>45475.923344907409</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="5">
+        <v>45486</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="E37" s="28" t="s">
         <v>115</v>
+      </c>
+      <c r="F37" s="34">
+        <v>45476.044374999998</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JD - updated participant list with who was paid for part 1
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farerilab/Documents/GitHub/WTP_Rejection_Choice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordansiegel/Documents/GitHub/WTP_Rejection_Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891EE0CE-8D0B-4D47-B5BE-07F882C075F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265B309C-4F53-8A4B-8303-5EA1C84ED434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="1700" windowWidth="30380" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1700" windowWidth="28800" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pilottotalparticipant_list!$K$1:$K$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="148">
   <si>
     <t>pavlovia_task</t>
   </si>
@@ -571,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -605,13 +618,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -623,6 +629,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,10 +856,10 @@
   <dimension ref="A1:X37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="180" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomRight" activeCell="E36" sqref="E36:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1294,37 +1301,36 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="24" t="s">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="5">
         <v>45467</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="10">
         <v>45466</v>
       </c>
-      <c r="G12" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="O12" s="26"/>
-      <c r="S12" s="27" t="s">
+      <c r="G12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S12" s="19" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1727,26 +1733,29 @@
         <v>142</v>
       </c>
       <c r="C25" s="16"/>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="34">
+      <c r="F25" s="29">
         <v>45475.893946759257</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>3</v>
       </c>
+      <c r="H25" s="30" t="s">
+        <v>3</v>
+      </c>
       <c r="I25" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="K25" s="31" t="s">
+      <c r="K25" s="26" t="s">
         <v>27</v>
       </c>
       <c r="O25" s="17"/>
-      <c r="S25" s="32"/>
+      <c r="S25" s="27"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
@@ -1758,16 +1767,19 @@
       <c r="C26" s="5">
         <v>45476</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="F26" s="34">
+      <c r="F26" s="29">
         <v>45475.933194444442</v>
       </c>
       <c r="G26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I26" s="4" t="s">
@@ -1790,16 +1802,19 @@
       <c r="C27" s="5">
         <v>45476</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="34">
+      <c r="F27" s="29">
         <v>45475.898773148147</v>
       </c>
       <c r="G27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I27" s="4" t="s">
@@ -1819,16 +1834,19 @@
       <c r="C28" s="5">
         <v>45477</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="F28" s="34">
+      <c r="F28" s="29">
         <v>45475.899189814816</v>
       </c>
       <c r="G28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I28" s="4" t="s">
@@ -1851,16 +1869,19 @@
       <c r="C29" s="5">
         <v>45478</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="34">
+      <c r="F29" s="29">
         <v>45475.907094907408</v>
       </c>
       <c r="G29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I29" s="4" t="s">
@@ -1880,18 +1901,19 @@
       <c r="C30" s="5">
         <v>45479</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="34">
+      <c r="F30" s="29">
         <v>45475.912314814814</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="H30" s="4"/>
       <c r="I30" s="4" t="s">
         <v>3</v>
       </c>
@@ -1912,16 +1934,19 @@
       <c r="C31" s="5">
         <v>45480</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="34">
+      <c r="F31" s="29">
         <v>45475.918715277781</v>
       </c>
       <c r="G31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H31" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I31" s="4" t="s">
@@ -1944,13 +1969,13 @@
       <c r="C32" s="5">
         <v>45481</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="F32" s="34">
+      <c r="F32" s="29">
         <v>45475.990833333337</v>
       </c>
       <c r="G32" s="4" t="s">
@@ -1976,16 +2001,19 @@
       <c r="C33" s="5">
         <v>45482</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E33" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="F33" s="34">
+      <c r="F33" s="29">
         <v>45476.090590277781</v>
       </c>
       <c r="G33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I33" s="4" t="s">
@@ -2005,16 +2033,19 @@
       <c r="C34" s="5">
         <v>45483</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="E34" s="28" t="s">
+      <c r="E34" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="F34" s="34">
+      <c r="F34" s="29">
         <v>45476.23265046296</v>
       </c>
       <c r="G34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I34" s="4" t="s">
@@ -2034,16 +2065,19 @@
       <c r="C35" s="5">
         <v>45484</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="F35" s="34">
+      <c r="F35" s="29">
         <v>45475.935532407406</v>
       </c>
       <c r="G35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I35" s="4" t="s">
@@ -2063,16 +2097,19 @@
       <c r="C36" s="5">
         <v>45485</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="E36" s="28" t="s">
+      <c r="E36" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="34">
+      <c r="F36" s="29">
         <v>45475.923344907409</v>
       </c>
       <c r="G36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I36" s="4" t="s">
@@ -2092,16 +2129,19 @@
       <c r="C37" s="5">
         <v>45486</v>
       </c>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="E37" s="28" t="s">
+      <c r="E37" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="F37" s="34">
+      <c r="F37" s="29">
         <v>45476.044374999998</v>
       </c>
       <c r="G37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I37" s="4" t="s">

</xml_diff>

<commit_message>
updated participant list with people with data, generated csvs for 667838be776b27f8705b6c3c (JD)
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordansiegel/Documents/GitHub/WTP_Rejection_Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265B309C-4F53-8A4B-8303-5EA1C84ED434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8774A7C2-E449-604E-939E-787A639E450B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1700" windowWidth="28800" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="1700" windowWidth="28800" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="152">
   <si>
     <t>pavlovia_task</t>
   </si>
@@ -479,7 +479,19 @@
     <t>photo 5 was a gif, replaced with photo 26; uploaded pictures from instagram app instead of internet browser, neds two more social experiences</t>
   </si>
   <si>
-    <t>getting more experiences</t>
+    <t>have data?</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -584,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -622,14 +634,17 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,13 +868,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X37"/>
+  <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="180" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E36" sqref="E36:E37"/>
+      <selection pane="bottomRight" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -868,23 +883,23 @@
     <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="4" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="10" customWidth="1"/>
-    <col min="7" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19" style="10" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="20" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="21.1640625" style="8" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="26" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="10" customWidth="1"/>
-    <col min="16" max="16" width="19.5" customWidth="1"/>
-    <col min="17" max="17" width="15.1640625" customWidth="1"/>
-    <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="19" width="103.33203125" style="12" customWidth="1"/>
-    <col min="20" max="23" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" customWidth="1"/>
+    <col min="16" max="16" width="19.5" style="10" customWidth="1"/>
+    <col min="17" max="17" width="19.5" customWidth="1"/>
+    <col min="18" max="18" width="15.1640625" customWidth="1"/>
+    <col min="19" max="19" width="16" customWidth="1"/>
+    <col min="20" max="20" width="103.33203125" style="12" customWidth="1"/>
+    <col min="21" max="24" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -921,44 +936,47 @@
       <c r="L1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="41" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
@@ -993,42 +1011,45 @@
       <c r="L2">
         <v>1</v>
       </c>
-      <c r="N2">
+      <c r="M2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="O2">
         <v>1</v>
       </c>
-      <c r="O2" s="10">
+      <c r="P2" s="10">
         <v>44875</v>
       </c>
-      <c r="P2">
-        <f>_xlfn.DAYS(O2,F2)</f>
+      <c r="Q2">
+        <f>_xlfn.DAYS(P2,F2)</f>
         <v>-518</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="R2" s="6">
         <v>2</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>0</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="T2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="4">
+      <c r="U2" s="4">
         <v>0</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>30</v>
       </c>
-      <c r="V2" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="W2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="X2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1057,8 +1078,11 @@
       <c r="K3" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M3" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>33</v>
       </c>
@@ -1087,8 +1111,11 @@
       <c r="K4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M4" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
@@ -1117,8 +1144,11 @@
       <c r="K5" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M5" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1147,8 +1177,11 @@
       <c r="K6" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M6" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
@@ -1177,8 +1210,11 @@
       <c r="K7" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M7" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>51</v>
       </c>
@@ -1207,8 +1243,11 @@
       <c r="K8" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M8" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>51</v>
       </c>
@@ -1237,8 +1276,11 @@
       <c r="K9" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M9" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>51</v>
       </c>
@@ -1267,8 +1309,11 @@
       <c r="K10" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M10" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>51</v>
       </c>
@@ -1297,11 +1342,14 @@
       <c r="K11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S11" s="19" t="s">
+      <c r="M11" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="T11" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>71</v>
       </c>
@@ -1330,11 +1378,14 @@
       <c r="K12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S12" s="19" t="s">
+      <c r="M12" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="T12" s="19" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>71</v>
       </c>
@@ -1365,8 +1416,11 @@
       <c r="K13" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M13" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>71</v>
       </c>
@@ -1397,8 +1451,11 @@
       <c r="K14" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M14" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>71</v>
       </c>
@@ -1426,11 +1483,14 @@
       <c r="K15" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="S15" s="12" t="s">
+      <c r="M15" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="T15" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>71</v>
       </c>
@@ -1461,11 +1521,14 @@
       <c r="K16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S16" s="19" t="s">
+      <c r="M16" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="T16" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>71</v>
       </c>
@@ -1499,8 +1562,11 @@
       <c r="L17" s="5">
         <v>45469</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M17" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
@@ -1528,12 +1594,15 @@
       <c r="K18" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O18" s="21"/>
-      <c r="S18" s="12" t="s">
+      <c r="M18" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="P18" s="21"/>
+      <c r="T18" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>71</v>
       </c>
@@ -1564,11 +1633,14 @@
       <c r="K19" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="S19" s="19" t="s">
+      <c r="M19" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="T19" s="19" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>71</v>
       </c>
@@ -1599,8 +1671,11 @@
       <c r="K20" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M20" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>71</v>
       </c>
@@ -1628,11 +1703,14 @@
       <c r="K21" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="S21" s="12" t="s">
+      <c r="M21" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="T21" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>71</v>
       </c>
@@ -1663,8 +1741,11 @@
       <c r="K22" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M22" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>71</v>
       </c>
@@ -1695,8 +1776,11 @@
       <c r="K23" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M23" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>71</v>
       </c>
@@ -1727,37 +1811,43 @@
       <c r="K24" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M24" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
         <v>142</v>
       </c>
       <c r="C25" s="16"/>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="27" t="s">
         <v>116</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F25" s="28">
         <v>45475.893946759257</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="30" t="s">
+      <c r="H25" s="29" t="s">
         <v>3</v>
       </c>
       <c r="I25" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="K25" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="O25" s="17"/>
-      <c r="S25" s="27"/>
-    </row>
-    <row r="26" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K25" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="P25" s="17"/>
+      <c r="T25" s="26"/>
+    </row>
+    <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>71</v>
       </c>
@@ -1767,13 +1857,13 @@
       <c r="C26" s="5">
         <v>45476</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="27" t="s">
         <v>123</v>
       </c>
       <c r="E26" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="28">
         <v>45475.933194444442</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -1785,14 +1875,17 @@
       <c r="I26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K26" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S26" s="12" t="s">
+      <c r="K26" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="T26" s="12" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>71</v>
       </c>
@@ -1802,13 +1895,13 @@
       <c r="C27" s="5">
         <v>45476</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="27" t="s">
         <v>117</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="28">
         <v>45475.898773148147</v>
       </c>
       <c r="G27" s="4" t="s">
@@ -1820,11 +1913,14 @@
       <c r="I27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K27" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K27" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>71</v>
       </c>
@@ -1834,13 +1930,13 @@
       <c r="C28" s="5">
         <v>45477</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="27" t="s">
         <v>118</v>
       </c>
       <c r="E28" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="28">
         <v>45475.899189814816</v>
       </c>
       <c r="G28" s="4" t="s">
@@ -1852,14 +1948,17 @@
       <c r="I28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K28" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S28" s="12" t="s">
+      <c r="K28" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="T28" s="12" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>71</v>
       </c>
@@ -1869,13 +1968,13 @@
       <c r="C29" s="5">
         <v>45478</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="27" t="s">
         <v>119</v>
       </c>
       <c r="E29" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="29">
+      <c r="F29" s="28">
         <v>45475.907094907408</v>
       </c>
       <c r="G29" s="4" t="s">
@@ -1887,11 +1986,14 @@
       <c r="I29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K29" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K29" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>71</v>
       </c>
@@ -1901,13 +2003,13 @@
       <c r="C30" s="5">
         <v>45479</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="27" t="s">
         <v>120</v>
       </c>
       <c r="E30" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="29">
+      <c r="F30" s="28">
         <v>45475.912314814814</v>
       </c>
       <c r="G30" s="4" t="s">
@@ -1917,14 +2019,17 @@
       <c r="I30" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K30" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="S30" s="12" t="s">
+      <c r="K30" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="T30" s="12" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>71</v>
       </c>
@@ -1934,13 +2039,13 @@
       <c r="C31" s="5">
         <v>45480</v>
       </c>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="27" t="s">
         <v>121</v>
       </c>
       <c r="E31" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="29">
+      <c r="F31" s="28">
         <v>45475.918715277781</v>
       </c>
       <c r="G31" s="4" t="s">
@@ -1952,14 +2057,17 @@
       <c r="I31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K31" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S31" s="12" t="s">
+      <c r="K31" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="T31" s="12" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>71</v>
       </c>
@@ -1969,13 +2077,13 @@
       <c r="C32" s="5">
         <v>45481</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="27" t="s">
         <v>128</v>
       </c>
       <c r="E32" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="F32" s="29">
+      <c r="F32" s="28">
         <v>45475.990833333337</v>
       </c>
       <c r="G32" s="4" t="s">
@@ -1987,11 +2095,14 @@
       <c r="K32" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="S32" s="12" t="s">
+      <c r="M32" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="T32" s="12" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>71</v>
       </c>
@@ -2001,13 +2112,13 @@
       <c r="C33" s="5">
         <v>45482</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="27" t="s">
         <v>126</v>
       </c>
       <c r="E33" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="F33" s="29">
+      <c r="F33" s="28">
         <v>45476.090590277781</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -2019,11 +2130,14 @@
       <c r="I33" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K33" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K33" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>71</v>
       </c>
@@ -2033,13 +2147,13 @@
       <c r="C34" s="5">
         <v>45483</v>
       </c>
-      <c r="D34" s="28" t="s">
+      <c r="D34" s="27" t="s">
         <v>127</v>
       </c>
       <c r="E34" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="F34" s="29">
+      <c r="F34" s="28">
         <v>45476.23265046296</v>
       </c>
       <c r="G34" s="4" t="s">
@@ -2051,11 +2165,14 @@
       <c r="I34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K34" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K34" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
         <v>71</v>
       </c>
@@ -2065,13 +2182,13 @@
       <c r="C35" s="5">
         <v>45484</v>
       </c>
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="27" t="s">
         <v>124</v>
       </c>
       <c r="E35" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="F35" s="29">
+      <c r="F35" s="28">
         <v>45475.935532407406</v>
       </c>
       <c r="G35" s="4" t="s">
@@ -2083,11 +2200,14 @@
       <c r="I35" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K35" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K35" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
         <v>71</v>
       </c>
@@ -2097,13 +2217,13 @@
       <c r="C36" s="5">
         <v>45485</v>
       </c>
-      <c r="D36" s="28" t="s">
+      <c r="D36" s="27" t="s">
         <v>122</v>
       </c>
       <c r="E36" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="29">
+      <c r="F36" s="28">
         <v>45475.923344907409</v>
       </c>
       <c r="G36" s="4" t="s">
@@ -2115,11 +2235,14 @@
       <c r="I36" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K36" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K36" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>71</v>
       </c>
@@ -2129,13 +2252,13 @@
       <c r="C37" s="5">
         <v>45486</v>
       </c>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="27" t="s">
         <v>125</v>
       </c>
       <c r="E37" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="F37" s="29">
+      <c r="F37" s="28">
         <v>45476.044374999998</v>
       </c>
       <c r="G37" s="4" t="s">
@@ -2147,8 +2270,11 @@
       <c r="I37" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K37" s="8" t="s">
-        <v>27</v>
+      <c r="K37" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added csvs for 10 participants from qualtrics (pretask and photoupload) and added raw images (JD)
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordansiegel/Documents/GitHub/WTP_Rejection_Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8774A7C2-E449-604E-939E-787A639E450B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97FB2DE-A342-2740-B79F-807FABDA4B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="1700" windowWidth="28800" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13740" yWindow="1720" windowWidth="28800" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="162">
   <si>
     <t>pavlovia_task</t>
   </si>
@@ -492,6 +492,36 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>6670297f1e47e468c3605ef4</t>
+  </si>
+  <si>
+    <t>5e49e45bc397b44533784587</t>
+  </si>
+  <si>
+    <t>6679bdceaa28479dfe378bb6</t>
+  </si>
+  <si>
+    <t>65c14027646a9bbfa89584c8</t>
+  </si>
+  <si>
+    <t>663ff3e539df6ec6f060f875</t>
+  </si>
+  <si>
+    <t>60c7fd00cce7a43663968b17</t>
+  </si>
+  <si>
+    <t>664d05ba68d4a45f6ba118a5</t>
+  </si>
+  <si>
+    <t>5d50feca50bdcf0001e8d38a</t>
+  </si>
+  <si>
+    <t>6496f9fbc2928ee6956ef623</t>
+  </si>
+  <si>
+    <t>63e55908254a436361a6787b</t>
   </si>
 </sst>
 </file>
@@ -501,7 +531,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -557,8 +587,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -577,12 +613,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -596,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -621,7 +651,6 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -634,17 +663,29 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,13 +909,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y37"/>
+  <dimension ref="A1:Y47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="180" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K31" sqref="K31"/>
+      <selection pane="bottomRight" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1326,7 +1367,7 @@
       <c r="D11" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>56</v>
       </c>
       <c r="F11" s="10">
@@ -1345,7 +1386,7 @@
       <c r="M11" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="T11" s="19" t="s">
+      <c r="T11" s="18" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1381,7 +1422,7 @@
       <c r="M12" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="T12" s="19" t="s">
+      <c r="T12" s="18" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1524,7 +1565,7 @@
       <c r="M16" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="T16" s="19" t="s">
+      <c r="T16" s="18" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1541,7 +1582,7 @@
       <c r="D17" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="21" t="s">
         <v>65</v>
       </c>
       <c r="F17" s="10">
@@ -1570,7 +1611,7 @@
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="19">
         <v>45467</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1579,7 +1620,7 @@
       <c r="E18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="20">
         <v>45466</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -1597,7 +1638,7 @@
       <c r="M18" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="P18" s="21"/>
+      <c r="P18" s="20"/>
       <c r="T18" s="12" t="s">
         <v>87</v>
       </c>
@@ -1636,7 +1677,7 @@
       <c r="M19" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="T19" s="19" t="s">
+      <c r="T19" s="18" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1815,37 +1856,40 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" t="s">
+    <row r="25" spans="1:20" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="27" t="s">
+      <c r="C25" s="30"/>
+      <c r="D25" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="28">
+      <c r="F25" s="32">
         <v>45475.893946759257</v>
       </c>
-      <c r="G25" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H25" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="K25" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="M25" s="29" t="s">
+      <c r="G25" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="P25" s="17"/>
-      <c r="T25" s="26"/>
+      <c r="P25" s="35"/>
+      <c r="T25" s="36"/>
     </row>
     <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
@@ -1857,13 +1901,13 @@
       <c r="C26" s="5">
         <v>45476</v>
       </c>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F26" s="28">
+      <c r="F26" s="27">
         <v>45475.933194444442</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -1875,7 +1919,7 @@
       <c r="I26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K26" s="30" t="s">
+      <c r="K26" s="28" t="s">
         <v>3</v>
       </c>
       <c r="M26" s="4" t="s">
@@ -1895,13 +1939,13 @@
       <c r="C27" s="5">
         <v>45476</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="28">
+      <c r="F27" s="27">
         <v>45475.898773148147</v>
       </c>
       <c r="G27" s="4" t="s">
@@ -1913,7 +1957,7 @@
       <c r="I27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K27" s="30" t="s">
+      <c r="K27" s="28" t="s">
         <v>3</v>
       </c>
       <c r="M27" s="4" t="s">
@@ -1930,13 +1974,13 @@
       <c r="C28" s="5">
         <v>45477</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28" s="27">
         <v>45475.899189814816</v>
       </c>
       <c r="G28" s="4" t="s">
@@ -1948,7 +1992,7 @@
       <c r="I28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K28" s="30" t="s">
+      <c r="K28" s="28" t="s">
         <v>3</v>
       </c>
       <c r="M28" s="4" t="s">
@@ -1968,13 +2012,13 @@
       <c r="C29" s="5">
         <v>45478</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="28">
+      <c r="F29" s="27">
         <v>45475.907094907408</v>
       </c>
       <c r="G29" s="4" t="s">
@@ -1986,7 +2030,7 @@
       <c r="I29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K29" s="30" t="s">
+      <c r="K29" s="28" t="s">
         <v>3</v>
       </c>
       <c r="M29" s="4" t="s">
@@ -2003,13 +2047,13 @@
       <c r="C30" s="5">
         <v>45479</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F30" s="27">
         <v>45475.912314814814</v>
       </c>
       <c r="G30" s="4" t="s">
@@ -2019,7 +2063,7 @@
       <c r="I30" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K30" s="30" t="s">
+      <c r="K30" s="28" t="s">
         <v>27</v>
       </c>
       <c r="M30" s="4" t="s">
@@ -2039,13 +2083,13 @@
       <c r="C31" s="5">
         <v>45480</v>
       </c>
-      <c r="D31" s="27" t="s">
+      <c r="D31" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="27">
         <v>45475.918715277781</v>
       </c>
       <c r="G31" s="4" t="s">
@@ -2057,7 +2101,7 @@
       <c r="I31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K31" s="30" t="s">
+      <c r="K31" s="28" t="s">
         <v>3</v>
       </c>
       <c r="M31" s="4" t="s">
@@ -2077,13 +2121,13 @@
       <c r="C32" s="5">
         <v>45481</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="D32" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="F32" s="28">
+      <c r="F32" s="27">
         <v>45475.990833333337</v>
       </c>
       <c r="G32" s="4" t="s">
@@ -2102,7 +2146,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>71</v>
       </c>
@@ -2112,13 +2156,13 @@
       <c r="C33" s="5">
         <v>45482</v>
       </c>
-      <c r="D33" s="27" t="s">
+      <c r="D33" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="E33" s="23" t="s">
+      <c r="E33" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="F33" s="28">
+      <c r="F33" s="27">
         <v>45476.090590277781</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -2130,14 +2174,14 @@
       <c r="I33" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K33" s="30" t="s">
+      <c r="K33" s="28" t="s">
         <v>3</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>71</v>
       </c>
@@ -2147,13 +2191,13 @@
       <c r="C34" s="5">
         <v>45483</v>
       </c>
-      <c r="D34" s="27" t="s">
+      <c r="D34" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="E34" s="23" t="s">
+      <c r="E34" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="F34" s="28">
+      <c r="F34" s="27">
         <v>45476.23265046296</v>
       </c>
       <c r="G34" s="4" t="s">
@@ -2165,14 +2209,14 @@
       <c r="I34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K34" s="30" t="s">
+      <c r="K34" s="28" t="s">
         <v>3</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
         <v>71</v>
       </c>
@@ -2182,13 +2226,13 @@
       <c r="C35" s="5">
         <v>45484</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="F35" s="28">
+      <c r="F35" s="27">
         <v>45475.935532407406</v>
       </c>
       <c r="G35" s="4" t="s">
@@ -2200,14 +2244,14 @@
       <c r="I35" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K35" s="30" t="s">
+      <c r="K35" s="28" t="s">
         <v>3</v>
       </c>
       <c r="M35" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
         <v>71</v>
       </c>
@@ -2217,13 +2261,13 @@
       <c r="C36" s="5">
         <v>45485</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="D36" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="28">
+      <c r="F36" s="27">
         <v>45475.923344907409</v>
       </c>
       <c r="G36" s="4" t="s">
@@ -2235,14 +2279,14 @@
       <c r="I36" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K36" s="30" t="s">
+      <c r="K36" s="28" t="s">
         <v>3</v>
       </c>
       <c r="M36" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>71</v>
       </c>
@@ -2252,13 +2296,13 @@
       <c r="C37" s="5">
         <v>45486</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="D37" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="E37" s="23" t="s">
+      <c r="E37" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="F37" s="28">
+      <c r="F37" s="27">
         <v>45476.044374999998</v>
       </c>
       <c r="G37" s="4" t="s">
@@ -2270,11 +2314,65 @@
       <c r="I37" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K37" s="30" t="s">
+      <c r="K37" s="28" t="s">
         <v>3</v>
       </c>
       <c r="M37" s="4" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E38" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" s="16"/>
+      <c r="K38" s="25"/>
+      <c r="P38" s="16"/>
+      <c r="T38" s="26"/>
+    </row>
+    <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E39" s="37" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E40" s="22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E41" s="37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E42" s="37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E43" s="37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E44" s="37" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E45" s="37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E46" s="37" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E47" s="38" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added WTP CSVS for 4 participants and highlighted who needs to send more
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farerilab/Documents/GitHub/WTP_Rejection_Choice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordansiegel/Documents/GitHub/WTP_Rejection_Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C31A62C-13DA-B246-A447-520D0530E68E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF81A73-A890-0C48-8685-5190421A7738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="5860" windowWidth="34140" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26560" yWindow="1940" windowWidth="28400" windowHeight="15160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pilottotalparticipant_list!$K$1:$K$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -586,10 +599,10 @@
     <t>changed photo 24 (alcohol) with photo 26</t>
   </si>
   <si>
-    <t>n- need more experiences (talking on the phone twice in social)</t>
-  </si>
-  <si>
-    <t>n-getting more experiences (put friends in nonsocial</t>
+    <t>getting more experiences</t>
+  </si>
+  <si>
+    <t>don’t see it</t>
   </si>
 </sst>
 </file>
@@ -694,7 +707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -734,21 +747,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -983,10 +983,10 @@
   <dimension ref="A1:Y48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="180" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L43" sqref="L43"/>
+      <selection pane="bottomRight" activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1927,40 +1927,38 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" t="s">
         <v>142</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="27" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F25" s="25">
         <v>45475.893946759257</v>
       </c>
-      <c r="G25" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="H25" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I25" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="K25" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="M25" s="31" t="s">
+      <c r="G25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="P25" s="33"/>
-      <c r="T25" s="34"/>
     </row>
     <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
@@ -1972,7 +1970,7 @@
       <c r="C26" s="5">
         <v>45476</v>
       </c>
-      <c r="D26" s="27" t="s">
+      <c r="D26" t="s">
         <v>123</v>
       </c>
       <c r="E26" s="23" t="s">
@@ -2010,7 +2008,7 @@
       <c r="C27" s="5">
         <v>45476</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" t="s">
         <v>117</v>
       </c>
       <c r="E27" s="22" t="s">
@@ -2045,7 +2043,7 @@
       <c r="C28" s="5">
         <v>45477</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" t="s">
         <v>118</v>
       </c>
       <c r="E28" s="22" t="s">
@@ -2083,7 +2081,7 @@
       <c r="C29" s="5">
         <v>45478</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" t="s">
         <v>119</v>
       </c>
       <c r="E29" s="22" t="s">
@@ -2118,7 +2116,7 @@
       <c r="C30" s="5">
         <v>45479</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" t="s">
         <v>120</v>
       </c>
       <c r="E30" s="22" t="s">
@@ -2154,7 +2152,7 @@
       <c r="C31" s="5">
         <v>45480</v>
       </c>
-      <c r="D31" s="27" t="s">
+      <c r="D31" t="s">
         <v>121</v>
       </c>
       <c r="E31" s="22" t="s">
@@ -2195,7 +2193,7 @@
       <c r="C32" s="5">
         <v>45481</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="D32" t="s">
         <v>128</v>
       </c>
       <c r="E32" s="22" t="s">
@@ -2233,7 +2231,7 @@
       <c r="C33" s="5">
         <v>45482</v>
       </c>
-      <c r="D33" s="27" t="s">
+      <c r="D33" t="s">
         <v>126</v>
       </c>
       <c r="E33" s="22" t="s">
@@ -2271,7 +2269,7 @@
       <c r="C34" s="5">
         <v>45483</v>
       </c>
-      <c r="D34" s="27" t="s">
+      <c r="D34" t="s">
         <v>127</v>
       </c>
       <c r="E34" s="22" t="s">
@@ -2309,7 +2307,7 @@
       <c r="C35" s="5">
         <v>45484</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" t="s">
         <v>124</v>
       </c>
       <c r="E35" s="22" t="s">
@@ -2347,7 +2345,7 @@
       <c r="C36" s="5">
         <v>45485</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="D36" t="s">
         <v>122</v>
       </c>
       <c r="E36" s="22" t="s">
@@ -2385,7 +2383,7 @@
       <c r="C37" s="5">
         <v>45486</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="D37" t="s">
         <v>125</v>
       </c>
       <c r="E37" s="22" t="s">
@@ -2420,27 +2418,27 @@
       <c r="B38" t="s">
         <v>173</v>
       </c>
-      <c r="C38" s="39">
+      <c r="C38" s="30">
         <v>45490</v>
       </c>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="14" t="s">
         <v>163</v>
       </c>
       <c r="E38" s="24" t="s">
         <v>152</v>
       </c>
       <c r="F38" s="16"/>
-      <c r="I38" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="K38" s="38" t="s">
-        <v>3</v>
+      <c r="I38" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="K38" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="P38" s="16"/>
       <c r="R38" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="T38" s="40" t="s">
+      <c r="T38" s="31" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2457,14 +2455,14 @@
       <c r="D39" t="s">
         <v>165</v>
       </c>
-      <c r="E39" s="35" t="s">
+      <c r="E39" s="27" t="s">
         <v>153</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K39" s="26" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="R39" t="s">
         <v>3</v>
@@ -2490,7 +2488,7 @@
         <v>3</v>
       </c>
       <c r="K40" s="26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R40" t="s">
         <v>3</v>
@@ -2509,7 +2507,7 @@
       <c r="D41" t="s">
         <v>166</v>
       </c>
-      <c r="E41" s="35" t="s">
+      <c r="E41" s="27" t="s">
         <v>155</v>
       </c>
       <c r="I41" s="4" t="s">
@@ -2538,14 +2536,14 @@
       <c r="D42" t="s">
         <v>167</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="27" t="s">
         <v>156</v>
       </c>
       <c r="I42" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K42" s="26" t="s">
-        <v>3</v>
+        <v>187</v>
       </c>
       <c r="R42" t="s">
         <v>3</v>
@@ -2567,14 +2565,14 @@
       <c r="D43" t="s">
         <v>168</v>
       </c>
-      <c r="E43" s="35" t="s">
+      <c r="E43" s="27" t="s">
         <v>157</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K43" s="26" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="R43" t="s">
         <v>3</v>
@@ -2593,14 +2591,14 @@
       <c r="D44" t="s">
         <v>169</v>
       </c>
-      <c r="E44" s="35" t="s">
+      <c r="E44" s="27" t="s">
         <v>158</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K44" s="26" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="R44" t="s">
         <v>3</v>
@@ -2619,14 +2617,14 @@
       <c r="D45" t="s">
         <v>170</v>
       </c>
-      <c r="E45" s="35" t="s">
+      <c r="E45" s="27" t="s">
         <v>159</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K45" s="26" t="s">
-        <v>3</v>
+        <v>188</v>
       </c>
       <c r="R45" t="s">
         <v>3</v>
@@ -2645,14 +2643,14 @@
       <c r="D46" t="s">
         <v>171</v>
       </c>
-      <c r="E46" s="35" t="s">
+      <c r="E46" s="27" t="s">
         <v>160</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K46" s="26" t="s">
-        <v>3</v>
+        <v>187</v>
       </c>
       <c r="R46" t="s">
         <v>3</v>
@@ -2674,14 +2672,14 @@
       <c r="D47" t="s">
         <v>172</v>
       </c>
-      <c r="E47" s="36" t="s">
+      <c r="E47" s="28" t="s">
         <v>161</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K47" s="26" t="s">
-        <v>3</v>
+        <v>187</v>
       </c>
       <c r="R47" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
(JD) edited participant list to reflect people we should have data for but we don't, noted who was added to the allow list
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordansiegel/Documents/GitHub/WTP_Rejection_Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF81A73-A890-0C48-8685-5190421A7738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9442D004-0153-3D40-B070-84026758A0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26560" yWindow="1940" windowWidth="28400" windowHeight="15160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37920" yWindow="1540" windowWidth="25060" windowHeight="15160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="188">
   <si>
     <t>pavlovia_task</t>
   </si>
@@ -600,9 +600,6 @@
   </si>
   <si>
     <t>getting more experiences</t>
-  </si>
-  <si>
-    <t>don’t see it</t>
   </si>
 </sst>
 </file>
@@ -675,7 +672,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -694,6 +691,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -707,7 +710,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -757,6 +760,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -983,10 +987,10 @@
   <dimension ref="A1:Y48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="180" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K48" sqref="K48"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2029,7 +2033,7 @@
       <c r="K27" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="M27" s="33" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2102,7 +2106,7 @@
       <c r="K29" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="M29" s="4" t="s">
+      <c r="M29" s="33" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2328,7 +2332,7 @@
       <c r="K35" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="M35" s="4" t="s">
+      <c r="M35" s="33" t="s">
         <v>148</v>
       </c>
       <c r="R35" t="s">
@@ -2366,7 +2370,7 @@
       <c r="K36" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="M36" s="4" t="s">
+      <c r="M36" s="33" t="s">
         <v>148</v>
       </c>
       <c r="R36" t="s">
@@ -2404,7 +2408,7 @@
       <c r="K37" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="M37" s="4" t="s">
+      <c r="M37" s="33" t="s">
         <v>148</v>
       </c>
       <c r="R37" t="s">
@@ -2624,7 +2628,7 @@
         <v>3</v>
       </c>
       <c r="K45" s="26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R45" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
JD-fixed WTP csv for one participant
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfareri/Documents/GitHub/WTP_Rejection_Choice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordansiegel/Documents/GitHub/WTP_Rejection_Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D61651-8D9A-134B-A89E-38D4A4EFF996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EA5A2D-1D07-0A42-B99A-20ADC028B30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="20240" windowHeight="22900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35260" yWindow="2100" windowWidth="28820" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="307">
   <si>
     <t>pavlovia_task</t>
   </si>
@@ -941,6 +941,21 @@
   </si>
   <si>
     <t>R_72bRN6zrzg5FrLG</t>
+  </si>
+  <si>
+    <t>why?</t>
+  </si>
+  <si>
+    <t>(need to get relationship specifics)</t>
+  </si>
+  <si>
+    <t>eligible</t>
+  </si>
+  <si>
+    <t>(needs manual link)</t>
+  </si>
+  <si>
+    <t>messaged, no response</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1072,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1112,6 +1127,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1338,10 +1354,10 @@
   <dimension ref="A1:Y1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C88" sqref="C88"/>
+      <selection pane="bottomRight" activeCell="M78" sqref="M78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3657,7 +3673,7 @@
         <v>3</v>
       </c>
       <c r="K71" s="19" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="M71" s="20" t="s">
         <v>265</v>
@@ -3727,9 +3743,11 @@
         <v>27</v>
       </c>
       <c r="K74" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="M74" s="31"/>
+        <v>3</v>
+      </c>
+      <c r="M74" s="31" t="s">
+        <v>303</v>
+      </c>
       <c r="P74" s="30"/>
       <c r="T74" s="32"/>
     </row>
@@ -3755,6 +3773,12 @@
       <c r="K75" s="19" t="s">
         <v>295</v>
       </c>
+      <c r="M75" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="T75" s="14" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="76" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
@@ -3776,7 +3800,10 @@
         <v>27</v>
       </c>
       <c r="K76" s="19" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="M76" s="38" t="s">
+        <v>304</v>
       </c>
       <c r="T76" s="14" t="s">
         <v>296</v>
@@ -3802,7 +3829,10 @@
         <v>27</v>
       </c>
       <c r="K77" s="19" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="M77" s="4" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="78" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3825,7 +3855,10 @@
         <v>27</v>
       </c>
       <c r="K78" s="19" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="M78" s="4" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="79" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3850,6 +3883,9 @@
       <c r="K79" s="19" t="s">
         <v>92</v>
       </c>
+      <c r="M79" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="T79" s="14" t="s">
         <v>298</v>
       </c>
@@ -3874,7 +3910,10 @@
         <v>27</v>
       </c>
       <c r="K80" s="19" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="M80" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3900,6 +3939,9 @@
       <c r="K81" s="19" t="s">
         <v>92</v>
       </c>
+      <c r="M81" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="T81" s="14" t="s">
         <v>299</v>
       </c>
@@ -3924,7 +3966,10 @@
         <v>27</v>
       </c>
       <c r="K82" s="19" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="M82" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="83" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3948,6 +3993,9 @@
       </c>
       <c r="K83" s="19" t="s">
         <v>295</v>
+      </c>
+      <c r="M83" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="T83" s="14" t="s">
         <v>297</v>

</xml_diff>